<commit_message>
Update shepherd_v2.4_Bill of Materials_packliste.xlsx
</commit_message>
<xml_diff>
--- a/PCBs/shepherd_cape_v2.4b/shepherd_v2.4_Bill of Materials_packliste.xlsx
+++ b/PCBs/shepherd_cape_v2.4b/shepherd_v2.4_Bill of Materials_packliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ingmo\Documents\GitHub\shepherd_v2_planning\PCBs\shepherd_cape_v2.4b\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E86E52-BE97-40B5-9883-CD7C67A125BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD52DB6F-2429-4A37-B6A2-1C6D24A9328B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4872" yWindow="3684" windowWidth="23316" windowHeight="21564" xr2:uid="{2F1582B1-F22C-4F74-AF12-6482AA6F50BB}"/>
+    <workbookView xWindow="18456" yWindow="780" windowWidth="23316" windowHeight="21564" xr2:uid="{2F1582B1-F22C-4F74-AF12-6482AA6F50BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-shepherd_v2" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="379">
   <si>
     <t>Comment</t>
   </si>
@@ -1167,13 +1167,19 @@
   </si>
   <si>
     <t>Kommentar</t>
+  </si>
+  <si>
+    <t>bestellt</t>
+  </si>
+  <si>
+    <t>critically low - nicht lieferbar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1190,6 +1196,23 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1238,17 +1261,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1566,10 +1591,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L64"/>
+  <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2777,7 +2802,7 @@
       </c>
       <c r="L32" s="7"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>193</v>
       </c>
@@ -2814,7 +2839,7 @@
       </c>
       <c r="L33" s="7"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>198</v>
       </c>
@@ -2851,7 +2876,7 @@
       </c>
       <c r="L34" s="7"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>205</v>
       </c>
@@ -2888,7 +2913,7 @@
       </c>
       <c r="L35" s="7"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>210</v>
       </c>
@@ -2921,13 +2946,16 @@
         <v>45</v>
       </c>
       <c r="K36" s="7">
-        <v>40</v>
-      </c>
-      <c r="L36" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="L36" s="11" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M36" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>215</v>
       </c>
@@ -2966,7 +2994,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>220</v>
       </c>
@@ -3005,7 +3033,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>225</v>
       </c>
@@ -3037,12 +3065,17 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="K39" s="7"/>
-      <c r="L39" s="8" t="s">
+      <c r="K39" s="7">
+        <v>100</v>
+      </c>
+      <c r="L39" s="11" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M39" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>230</v>
       </c>
@@ -3081,7 +3114,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>235</v>
       </c>
@@ -3120,7 +3153,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>240</v>
       </c>
@@ -3157,7 +3190,7 @@
       </c>
       <c r="L42" s="7"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>245</v>
       </c>
@@ -3194,7 +3227,7 @@
       </c>
       <c r="L43" s="7"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>250</v>
       </c>
@@ -3231,7 +3264,7 @@
       </c>
       <c r="L44" s="7"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>255</v>
       </c>
@@ -3268,7 +3301,7 @@
       </c>
       <c r="L45" s="7"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>261</v>
       </c>
@@ -3305,7 +3338,7 @@
       </c>
       <c r="L46" s="7"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>267</v>
       </c>
@@ -3342,7 +3375,7 @@
       </c>
       <c r="L47" s="7"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>273</v>
       </c>
@@ -3379,7 +3412,7 @@
       </c>
       <c r="L48" s="7"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>279</v>
       </c>
@@ -3415,10 +3448,10 @@
         <v>368</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>284</v>
       </c>
@@ -3457,7 +3490,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>289</v>
       </c>
@@ -3494,7 +3527,7 @@
       </c>
       <c r="L51" s="7"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>295</v>
       </c>
@@ -3526,12 +3559,17 @@
         <f t="shared" si="0"/>
         <v>135</v>
       </c>
-      <c r="K52" s="7"/>
-      <c r="L52" s="8" t="s">
+      <c r="K52" s="7">
+        <v>160</v>
+      </c>
+      <c r="L52" s="10" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M52" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>301</v>
       </c>
@@ -3568,7 +3606,7 @@
       </c>
       <c r="L53" s="7"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>308</v>
       </c>
@@ -3605,7 +3643,7 @@
       </c>
       <c r="L54" s="7"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>314</v>
       </c>
@@ -3642,7 +3680,7 @@
       </c>
       <c r="L55" s="7"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>319</v>
       </c>
@@ -3679,7 +3717,7 @@
       </c>
       <c r="L56" s="7"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>324</v>
       </c>
@@ -3716,7 +3754,7 @@
       </c>
       <c r="L57" s="7"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>330</v>
       </c>
@@ -3753,7 +3791,7 @@
       </c>
       <c r="L58" s="7"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>335</v>
       </c>
@@ -3790,7 +3828,7 @@
       </c>
       <c r="L59" s="7"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>339</v>
       </c>
@@ -3827,7 +3865,7 @@
       </c>
       <c r="L60" s="7"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>344</v>
       </c>
@@ -3864,7 +3902,7 @@
       </c>
       <c r="L61" s="7"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>348</v>
       </c>
@@ -3901,7 +3939,7 @@
       </c>
       <c r="L62" s="7"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>353</v>
       </c>
@@ -3938,7 +3976,7 @@
       </c>
       <c r="L63" s="7"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>359</v>
       </c>

</xml_diff>